<commit_message>
oop in the player & new inputs :)
</commit_message>
<xml_diff>
--- a/real_songs_data.xlsx
+++ b/real_songs_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,124 +484,250 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>alarm.mp3</t>
+          <t>perfect-beauty-191271.mp3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2607891156462585</v>
+        <v>7.3412</v>
       </c>
       <c r="C3" t="n">
-        <v>15.64734693877551</v>
+        <v>440.472</v>
       </c>
       <c r="D3" t="n">
-        <v>15.64734693877551</v>
+        <v>440.472</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[107.66601562]</t>
+          <t>[161.49902344]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>testfile3.mp3</t>
+          <t>alarm.mp3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2573061224489796</v>
+        <v>0.2607891156462585</v>
       </c>
       <c r="C4" t="n">
-        <v>15.43836734693878</v>
+        <v>15.64734693877551</v>
       </c>
       <c r="D4" t="n">
-        <v>15.43836734693878</v>
+        <v>15.64734693877551</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[64.59960938]</t>
+          <t>[107.66601562]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>testfile2.mp3</t>
+          <t>endless-horizons-223627.mp3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.618448979591837</v>
+        <v>1.7812</v>
       </c>
       <c r="C5" t="n">
-        <v>277.1069387755102</v>
+        <v>106.872</v>
       </c>
       <c r="D5" t="n">
-        <v>277.1069387755102</v>
+        <v>106.872</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[129.19921875]</t>
+          <t>[117.45383523]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>electroni_middle.mp3</t>
+          <t>testfile3.mp3</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3091156462585034</v>
+        <v>0.2573061224489796</v>
       </c>
       <c r="C6" t="n">
-        <v>18.5469387755102</v>
+        <v>15.43836734693878</v>
       </c>
       <c r="D6" t="n">
-        <v>18.5469387755102</v>
+        <v>15.43836734693878</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[89.10290948]</t>
+          <t>[64.59960938]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>violin.mp3</t>
+          <t>lotus-sky-dreams-216049.mp3</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3474285714285715</v>
+        <v>2.4112</v>
       </c>
       <c r="C7" t="n">
-        <v>20.84571428571429</v>
+        <v>144.672</v>
       </c>
       <c r="D7" t="n">
-        <v>20.84571428571429</v>
+        <v>144.672</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[107.66601562]</t>
+          <t>[99.38401442]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>testfile2.mp3</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.618448979591837</v>
+      </c>
+      <c r="C8" t="n">
+        <v>277.1069387755102</v>
+      </c>
+      <c r="D8" t="n">
+        <v>277.1069387755102</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[129.19921875]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>electroni_middle.mp3</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.3091156462585034</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18.5469387755102</v>
+      </c>
+      <c r="D9" t="n">
+        <v>18.5469387755102</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[89.10290948]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>violin.mp3</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.3474285714285715</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20.84571428571429</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20.84571428571429</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[107.66601562]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>night-detective-226857.mp3</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.9332</v>
+      </c>
+      <c r="C11" t="n">
+        <v>115.992</v>
+      </c>
+      <c r="D11" t="n">
+        <v>115.992</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[73.828125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>titanium.mp3</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="C12" t="n">
+        <v>106.2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>106.2</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[64.59960938]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>island-breeze-214305.mp3</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.5108</v>
+      </c>
+      <c r="C13" t="n">
+        <v>90.648</v>
+      </c>
+      <c r="D13" t="n">
+        <v>90.648</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[107.66601562]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>alarm2.mp3</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B14" t="n">
         <v>0.6743945578231293</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C14" t="n">
         <v>40.46367346938776</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D14" t="n">
         <v>40.46367346938776</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>[129.19921875]</t>
         </is>

</xml_diff>